<commit_message>
Evidence for tasks A1-A6
</commit_message>
<xml_diff>
--- a/IAmScRay/evidence.xlsx
+++ b/IAmScRay/evidence.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\^-^\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="9338" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9375" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t>TeamName</t>
   </si>
@@ -75,33 +75,15 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
     <t>nft id</t>
   </si>
   <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
     <t>ibc class on chain</t>
   </si>
   <si>
@@ -142,13 +124,55 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>717563F5AE78BA5CC0AF75D78A9E53135B145E82ABB8D7C3B4404EF7B6AC5C6A</t>
+  </si>
+  <si>
+    <t>denomSCR001</t>
+  </si>
+  <si>
+    <t>FB33844034957A742B6AEB4F4E28E11C080CA5C6AE263EA2BD2E7CCABF3AC755</t>
+  </si>
+  <si>
+    <t>nSCR001</t>
+  </si>
+  <si>
+    <t>nSCR002</t>
+  </si>
+  <si>
+    <t>9E685D7B06041447544DEC1FACB9C470BDF3D623D8594440822BA3A8691BB4FE</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>ECA61888DA686C33E26FD052A4119D8B0FE1CA4D76A92C394CABE827FE3763ED</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>ibc/9D482D84636D6D84DCAB9E59A8B0AEBC216B46A94D05BDD1496527FB139CEA8A</t>
+  </si>
+  <si>
+    <t>E86B319D6AEB7719057A845F3C76205785ADAEFAE3405ADECEE9BDBD55B261FD</t>
+  </si>
+  <si>
+    <t>31A29CE0048FEE0B4DB01D62CE33380014007ABD6106B3E70D327A10BD9E1336</t>
+  </si>
+  <si>
+    <t>stars1rracsh93v5ldqjxg03ld0r86qeugrakf63h76kuymr2jngql50tstm506d</t>
+  </si>
+  <si>
+    <t>0CE825E7622A04C81104F8FB70F9E5D904F73B6916E7A616C36F4303B60D29CA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -166,6 +190,20 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -200,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -212,6 +250,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -559,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
@@ -603,29 +648,29 @@
     </row>
     <row r="2" spans="1:8" ht="13.5">
       <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>32</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -649,15 +694,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -682,15 +727,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -715,15 +760,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -748,15 +793,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -781,25 +826,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -824,25 +869,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -867,25 +912,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -910,25 +955,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -953,25 +998,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -996,25 +1041,25 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1027,11 +1072,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="17.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.5">
+      <c r="A2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="17.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.5">
@@ -1039,101 +1119,68 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.5">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13.5">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.5">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="13.5">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13.5">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1157,12 +1204,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.45" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1192,12 +1239,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1227,12 +1274,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1262,12 +1309,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1282,9 +1329,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -1300,18 +1349,29 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.5">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
+      <c r="A2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13.5">
+      <c r="A3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1324,7 +1384,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -1340,197 +1402,203 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.5">
+      <c r="A2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="17.86328125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.5">
+      <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="17.86328125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+    <col min="2" max="2" width="17.9296875" customWidth="1"/>
+    <col min="3" max="3" width="16.265625" customWidth="1"/>
+    <col min="4" max="4" width="14.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="2" width="17.86328125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="2" width="17.86328125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="13.5">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="17.86328125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="16.265625" customWidth="1"/>
-    <col min="4" max="4" width="14.3984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="13.5">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1555,15 +1623,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Evidence for tasks A7-A10, B1-B2
Tasks A11-A20 are to be uploaded a bit later.
</commit_message>
<xml_diff>
--- a/IAmScRay/evidence.xlsx
+++ b/IAmScRay/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9375" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9375" tabRatio="500" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="54">
   <si>
     <t>TeamName</t>
   </si>
@@ -166,6 +166,45 @@
   </si>
   <si>
     <t>0CE825E7622A04C81104F8FB70F9E5D904F73B6916E7A616C36F4303B60D29CA</t>
+  </si>
+  <si>
+    <t>nSCR003</t>
+  </si>
+  <si>
+    <t>ibc/F280FCB9F55A0AF42D862B119300753A40E1B785F1E05A2AA25FAE29823E10AB</t>
+  </si>
+  <si>
+    <t>nSCR004</t>
+  </si>
+  <si>
+    <t>ibc/97AB6FD728F6E352554E257CE31F9CB94046DB484007854F1C7EB242C00AB394</t>
+  </si>
+  <si>
+    <t>ibc/34D1A04099AE81F7045226A6E3B51CC3C9006BE66328ABFEF737098EB4712D66</t>
+  </si>
+  <si>
+    <t>nSCR005</t>
+  </si>
+  <si>
+    <t>ibc/36C056BA51049EE084B935CA687FFF46548E3E8C31B2D0E3AB619593797EFC93</t>
+  </si>
+  <si>
+    <t>nSCR006</t>
+  </si>
+  <si>
+    <t>nSCR007</t>
+  </si>
+  <si>
+    <t>1A793EDE598458783035C26B192B8DC1EA18D891160903796368B469459B85DB</t>
+  </si>
+  <si>
+    <t>AEFE4EECED23F73C9BD8C38346D3B15B72BBF11FBCFE7A2611E0EE8BD1BC9141</t>
+  </si>
+  <si>
+    <t>65B3EDDDF1A63585565425656F4C2ED2B98FD05FD36BD429773D17B1D83FFD82</t>
+  </si>
+  <si>
+    <t>6CB6BB6692A10C2AF67A16B3F21F8E0EB704613FDD0E41B29F506B812102C97D</t>
   </si>
 </sst>
 </file>
@@ -682,7 +721,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.5">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.5">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -702,16 +813,16 @@
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -744,72 +855,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.5">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.5">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
@@ -1073,7 +1118,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
@@ -1193,7 +1238,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="12.75"/>
   <sheetData>
@@ -1204,12 +1251,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.45" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1227,7 +1274,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="12.75"/>
@@ -1239,12 +1286,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1379,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
@@ -1480,7 +1527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1578,7 +1625,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -1595,10 +1644,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1611,7 +1660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -1628,10 +1679,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Evidence for tasks A7-A10, B1 & B2, B5-B7
Evidence for tasks A11-A20 is to be uploaded later.
</commit_message>
<xml_diff>
--- a/IAmScRay/evidence.xlsx
+++ b/IAmScRay/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9375" tabRatio="500" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9375" tabRatio="500" firstSheet="9" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -37,13 +37,14 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="58">
   <si>
     <t>TeamName</t>
   </si>
@@ -96,12 +97,6 @@
     <t>tx hash on that chain	chain id</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>MultVR</t>
   </si>
   <si>
@@ -205,6 +200,24 @@
   </si>
   <si>
     <t>6CB6BB6692A10C2AF67A16B3F21F8E0EB704613FDD0E41B29F506B812102C97D</t>
+  </si>
+  <si>
+    <t>AB4AACAAE21742FF36B0F1A2CE94CD012A13DA031443798D8BFFC719F2261B44</t>
+  </si>
+  <si>
+    <t>99D9B84B978A1EEABACB4592F2F72A228D7709568A8AC4A4462B3FBDB4D97942</t>
+  </si>
+  <si>
+    <t>695DBC2F67FE0D7FEDD7E352C6B9B05D973BF1E2E7F4882B09D4EA5841069A01</t>
+  </si>
+  <si>
+    <t>0A67FD012F0DB14149AC0E1C12F466C50274ABFCFCF49F70DC2BF286D045235C</t>
+  </si>
+  <si>
+    <t>70E458DB1FB2D12E5B0E3E744F7BC4FAC6984FECC6EDF424D75F92C58ECE1A79</t>
+  </si>
+  <si>
+    <t>24DA52E5F18C1D454F7C0467A4F6BA5B66DC2A3326FC77C2E2AE39B083EF5EE1</t>
   </si>
 </sst>
 </file>
@@ -277,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -298,6 +311,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -687,28 +701,28 @@
     </row>
     <row r="2" spans="1:8" ht="13.5">
       <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="H2" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -740,45 +754,45 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.5">
+      <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.5">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -813,7 +827,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1136,10 +1150,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1195,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="O1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -1251,12 +1265,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.45" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1286,12 +1300,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1309,7 +1323,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="12.75"/>
@@ -1321,12 +1335,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1344,7 +1358,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="12.75"/>
@@ -1356,12 +1370,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1374,6 +1388,36 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="13.5">
+      <c r="A2" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="13.5">
+      <c r="A3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
@@ -1401,24 +1445,24 @@
     </row>
     <row r="2" spans="1:3" ht="13.5">
       <c r="A2" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.5">
       <c r="A3" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1457,16 +1501,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1505,16 +1549,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1553,16 +1597,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1576,7 +1620,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
@@ -1603,16 +1647,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1644,10 +1688,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1679,10 +1723,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Evidence for tasks A11-A20
</commit_message>
<xml_diff>
--- a/IAmScRay/evidence.xlsx
+++ b/IAmScRay/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9375" tabRatio="500" firstSheet="9" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9375" tabRatio="500" firstSheet="16" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="98">
   <si>
     <t>TeamName</t>
   </si>
@@ -82,12 +82,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
     <t>tx hash on that chain</t>
   </si>
   <si>
@@ -218,6 +212,132 @@
   </si>
   <si>
     <t>24DA52E5F18C1D454F7C0467A4F6BA5B66DC2A3326FC77C2E2AE39B083EF5EE1</t>
+  </si>
+  <si>
+    <t>ibc/12293CFAC83C2DF0DE89D73B9F1686F0AE829338371EE904131485F75CB5EB6D</t>
+  </si>
+  <si>
+    <t>ibc/F798D839824ADCB98D8D1E3EE49E9923CAB139DFD0692B6D2E393CCEA9F8281B</t>
+  </si>
+  <si>
+    <t>nSCR008</t>
+  </si>
+  <si>
+    <t>DBB35FF7CFB969634E097589C65F05DD8C3BD19628A44A5756E7EB04A164B0AE</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>536E0DF4AC9F2A63FD9236CA66903F5AA67EF9D49F55F1DB3A41E357972A940C</t>
+  </si>
+  <si>
+    <t>66688AF8384AA27BAD9927FAFA39CE7894D3564DA9AAC0BF1B5C8A5069D717A5</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>EF3D0E8511D534FFBC1C1FE070B4DDD9852DA7E4BCD6C4A1909611F06A1C5B1A</t>
+  </si>
+  <si>
+    <t>3E2CEEA2DCFD195D2BCC761A723924FB739B1EC551211D7608FC04F6788B87DB</t>
+  </si>
+  <si>
+    <t>7C8633DB72B7CC5CD0D96158CFCDDA970AFE30D560DF8BA0E3BF6C2D52D5C999</t>
+  </si>
+  <si>
+    <t>916060DC928571835F13B5D4EF5F97C74568F76E71160F09EAEC87B618268D6D</t>
+  </si>
+  <si>
+    <t>386F5CCB8F5CCF9233F7926C11ECFE71C9BED88F07E36111A8523939713FE7DC</t>
+  </si>
+  <si>
+    <t>833D786BABBA5EE663D37E269490488C803FDDF5410F33A55C7B5F6D608CB0C4</t>
+  </si>
+  <si>
+    <t>67402AF8DD0396238C83B35DB88A7ABD67BB97FB1F8E7BCEDF438C55878DD2F2</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>D722B5A3C0236822EB0280A088125BD090918BBA5CBCE28CB38460178CE6AD38</t>
+  </si>
+  <si>
+    <t>816BCAA431C4C9E3B7C7C75C9587204BA84DD8077DE530B2FC290C373659DDC4</t>
+  </si>
+  <si>
+    <t>EB45DC9B4AA93F291871364BF575DCFA2638E806914CA9A70065CD9F9E1FFCD5</t>
+  </si>
+  <si>
+    <t>CDAED108FAB715AA5D28674294DC5B911D01A548BAC2662698822902EE9C0E16</t>
+  </si>
+  <si>
+    <t>28342E56C696D89B67E331238F1465E3FEC04934EA3463838283111D28300E94</t>
+  </si>
+  <si>
+    <t>98864727B63C59F8F4610C650CD9AE0F3EFEBC16EF5C0B2F91CBD0417093D889</t>
+  </si>
+  <si>
+    <t>66231F26D7B44B66FB0EF6732B1A8B452568BF997F17059A37C34CDA0C615C8F</t>
+  </si>
+  <si>
+    <t>0CEF4DCEA43AB9D5F93378909F3D978CB011A021502974A7772D42F6E1F0E167</t>
+  </si>
+  <si>
+    <t>7C041463DADA5B38F112B98E906333859C18A1C838ED0C76EEAD717E8C8B33D1</t>
+  </si>
+  <si>
+    <t>65EDA530C04DFEC6D00D639B01027871183D506CE1A9AF79332BEE93935DF9A7</t>
+  </si>
+  <si>
+    <t>0C4808210481AF9E20E446E644A69226277529131E4988DC9D8E84FD9268E0A0</t>
+  </si>
+  <si>
+    <t>75920F9676D8E63E02301FA0F41F8B1BD591F4BE9A91A601ECB3F062BB7BD848</t>
+  </si>
+  <si>
+    <t>C4BEAD3088470B30C4C2D5B53E880082F8B6893022042515C6D7D3547A38C4AF</t>
+  </si>
+  <si>
+    <t>EB834BED2E429A73231ED032D715DF888F17CD240F187D2C7E07B460ECE0A140</t>
+  </si>
+  <si>
+    <t>64EE35C4FE0075E2C17225B1E134661CE63A39D0134732236AB150228D84EB73</t>
+  </si>
+  <si>
+    <t>25D8677C52BF449693AB3D24EA8DDC29B9C27EA6251787393317CEEED8F6BA6F</t>
+  </si>
+  <si>
+    <t>2B60405F534A89D1982EC5CAF626093B1CEADABD041922B358A6F54F1C61A109</t>
+  </si>
+  <si>
+    <t>0816E501A384AC9A5BB1B5379432E62FD3A1E5B1B7D7AC4DEEFE1CF993B99F63</t>
+  </si>
+  <si>
+    <t>AA45B026D5BBF4A82651BBA66C66A36290D90610D622F07E4A475588F4B1C9B6</t>
+  </si>
+  <si>
+    <t>934646DBD291F3CC46E15BDF7CAC730625A25383738C3DA24C56DB61251D4335</t>
+  </si>
+  <si>
+    <t>BF40994A2A4CFC2D4DEF730B762B07180EA9677A99F037E6CB02AAE1C8A3F3F1</t>
+  </si>
+  <si>
+    <t>7158FA8918F242E1AD4B039A8D4158CC86BCD5A5F5FA489D0ED0A87DDC5F9942</t>
+  </si>
+  <si>
+    <t>7F2840C2A465FC36E2E9DA53DD268B173BBC6AE21B601EC4C9DB3DE7392A57B1</t>
+  </si>
+  <si>
+    <t>AE1E0131387D181FEAF9218638D07F356028E5B459ECFE8795654D57FE077701</t>
+  </si>
+  <si>
+    <t>942B3233FBA8699A38E650865C34C4C7F0DD38BDD0FBAD5E41688907CC7F6593</t>
+  </si>
+  <si>
+    <t>C6B7159B2D43D7BE2509A36E5F22243A39165BEB6058BA8AE5ACAA17FF92A5DB</t>
   </si>
 </sst>
 </file>
@@ -290,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -312,6 +432,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -701,28 +822,28 @@
     </row>
     <row r="2" spans="1:8" ht="13.5">
       <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="D2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="H2" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -754,10 +875,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -789,10 +910,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -806,7 +927,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
@@ -824,10 +945,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -857,10 +980,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -871,9 +994,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -890,20 +1015,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5">
+      <c r="A5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -914,9 +1053,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -933,20 +1074,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5">
+      <c r="A5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -957,9 +1112,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -976,20 +1133,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5">
+      <c r="A5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1000,9 +1171,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -1011,7 +1184,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="13.5">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -1019,20 +1192,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5">
+      <c r="A5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1043,9 +1230,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -1062,20 +1251,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5">
+      <c r="A5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1086,9 +1289,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -1105,20 +1310,34 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5">
+      <c r="A5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1150,10 +1369,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1164,9 +1383,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
@@ -1181,22 +1402,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.5">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="13.5">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13.5">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1207,39 +1458,89 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0"/>
+  <dimension ref="A1:P7"/>
+  <sheetViews>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.5">
+    <row r="1" spans="1:16" ht="13.5">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.5">
+      <c r="O1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="13.5">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="13.5">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="13.5">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13.5">
+      <c r="O3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="P3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="13.5">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="P4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="O5" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="13.5">
+      <c r="O6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="P6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="O7" t="s">
+        <v>91</v>
+      </c>
+      <c r="P7" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1265,12 +1566,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.45" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1300,12 +1601,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1335,12 +1636,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1370,12 +1671,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1405,12 +1706,12 @@
     </row>
     <row r="2" spans="1:1" ht="13.5">
       <c r="A2" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.5">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1445,24 +1746,24 @@
     </row>
     <row r="2" spans="1:3" ht="13.5">
       <c r="A2" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.5">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1501,16 +1802,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1549,16 +1850,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1597,16 +1898,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1647,16 +1948,16 @@
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1688,10 +1989,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1723,10 +2024,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>